<commit_message>
Changes to be committed: 	modified:   .gitignore 	modified:   System Administrator_jobs.xlsx 	modified:   scratch
</commit_message>
<xml_diff>
--- a/System Administrator_jobs.xlsx
+++ b/System Administrator_jobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>Job Title</t>
   </si>
@@ -29,6 +29,37 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>Windows System Administrator</t>
+  </si>
+  <si>
+    <t>Asset Inventories, Inc.</t>
+  </si>
+  <si>
+    <t>New York, NY 10022 
+(Midtown area)</t>
+  </si>
+  <si>
+    <t>$94,087 - $103,055 a year
+Full-time
+Monday to Friday
++2</t>
+  </si>
+  <si>
+    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0Dg1PXRVsEYTLQ3LoznZ18-3yKIkD2vTai76bYwQ_bmGHsM0AvZ4FWgK6JlVJi5GZpJObXX25wKRZBrDGrnjr8-PwMQpLa6nVKu_-BwQtFP5hvHer7TRW-GYx0XVOZjeoU6dPkvtBkEoJbj-rWIVhu5Aj6WPIOQTgKXUHqsKVQStj7Rl84uksq3zEGfAizZGOX4sBE0liI62py0QAxW90MfxCv6tptzLVQaCp6zM9jgi9fICcLWyJUOjQ8H3uOQB1sx5pSGwkUThY4hpyO1AdxQQiTFlC1wRIq7a5ixwb4Pj0tGCtLiQYa7vQu9_hNB2qFJX7yD6vabgm7WO3t5yPGVfM4V6HuWkyTDSUkBCDXZj4blXrBkQ8C8mIF0IVJrL7QLV8Ae9fZOfO4-JTGAEhTVYmqerZO_6r6s_GFFZHmgfPu-vMd_qW_ovZLgNlKgp5nXE0mNOpub9vy2DkKAa8H9VZz6xNNu1McoO9qA71v6KE7qlvqRouYTCDYllib91x-8xHB-fXBUM3ZiZWkHWtDPmouRhv6a2aHZCh75JmhxcAOuSY9QOmWbYRgpawxKCss=&amp;xkcb=SoBT-_M3QegCKEWxBB0JbzkdCdPP&amp;p=0&amp;fvj=1&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>Linux System Engineer</t>
+  </si>
+  <si>
+    <t>$100,000 - $120,000 a year
+Full-time
+Monday to Friday
++2</t>
+  </si>
+  <si>
+    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0Dg1PXRVsEYTLQ3LoznZ18-3yKIkD2vTai76bYwQ_bmGHsM0AvZ4FWgnOxKIaJeSNnUdhaIHickuqPxg7ijsVvSvqfust0yko_iViu2v4TL2Ya1QIPI2AobC6ewvLwkUASOZinT_chjl0SNS5h_K55eA-cTybGglaRjGFoVjbarkYwPYfC2avdQAVlxTEkXlUesayE9EfeDmv20bolh5BEXAg7H-n3jQxZvcfjqQT9EtoQjP2BlzabSXyWk3Q_wU56I1Kr9icxMzT-w1YbhbuO4Mf7hpXG9790MGF9APcwPsKnV5-lDKjJuAN7T3mqSczSxXuCvXK2ccAnCzz-q-Y7ZeqS84_hLc9r2WFRC3KOa4K4YmOAtlrLAMKh9lRgeL3RCGRMHQwJS_4S2RTw33J2UOXGJmab245L9iz7C2gdlVRYAa-AsrC0MIqAmqK1kWZcagYo2rm7xTTGYFVCPC1_RJwG5cTZT1kO7IXEAxTAcSHRLxwMcsQkAjjqnUMmMMijx_gbk20zSURHxK4AHIRo2WoAiTs7B0_A8keqMRu5Z2eawRQfphGwEX7sDfNfTdFc=&amp;xkcb=SoDn-_M3QegCKEWxBB0IbzkdCdPP&amp;p=1&amp;fvj=1&amp;vjs=3</t>
   </si>
   <si>
     <t>Network and System Administrator</t>
@@ -46,24 +77,23 @@
 +3</t>
   </si>
   <si>
-    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CJvkUx1eZm87KuDgDx4Kuda_e0vlCxMB0uCCekvXkAFguDtuIQ7Y2XfpoRge0S6GHPmD1_X4x0jh3_WDfGD6_-VY6pBminZrzKoGKjyIuFM6q8bQezZoIVQsoadWapqvtNWbU1G11g65HjWP-poKc4UXq-KrSB9V67g9ARca01ty4QrnTZTBsCiAHKTFhQE8K3UIPfcztiSbJ283xDF8G5ICQlH1Rn-ET_2SNHdChyn2Mygna9JW9Q0jP_XCv2oI5d2n4eKXPk_T5yYVIuCLvYcJm5w6bx4IEMo14ynVE35V6T1nQ7YbfrQJZGO8cbBc8c5q0Ny6u3HzDLmkuodA7raC0AHsRaeYyaUowm5HhrnA-bX2me32dJYxykl9R7WKeiwDLli5_tYzr6B7gFaRoWqz3hyAR1FTmkIdxVgQACBXtP6p93gZzdDuhVYd3T7_KWAVIEhBN6SJqr23zc-M71uGqpinaiNH4zPC--55ymvgAS38FAJFSRr4ASQ7WcU0ZeZx_n-gv-2_W3t5MrnJUgYHviFl7_Y1JI3ZaIPqfmWZ0vUzGQYTDFuI_T6bUPDqZGtBJKDQhCKA==&amp;xkcb=SoBP-_M3Qd5AiLQgXJ0LbzkdCdPP&amp;p=0&amp;fvj=1&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>vCIO / Managed Services System Administrator</t>
-  </si>
-  <si>
-    <t>Bowman Williams</t>
-  </si>
-  <si>
-    <t>New York, NY
-+3 locations</t>
+    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CJvkUx1eZm87KuDgDx4Kuda_e0vlCxMB0uCCekvXkAFguDtuIQ7Y2XfpoRge0S6GHPmD1_X4x0jh3_WDfGD6_-VY6pBminZrzKoGKjyIuFM6q8bQezZoIVQsoadWapqvtNWbU1G11g65HjWP-poKc4UXq-KrSB9V67g9ARca01t_PbSNQoOSMKcONQK9cnK_UxBiRRS_1VCQCYIKszu0rhwlpWSxbBif8Xh1doAB1q2G5l4LxJQqygdlj6hRwoN2DWgKP8YP2oT53HblkcE040RGtJVlhAdLSBay2R2GfoxRHjhnIFx_WGNWUWTZZNVuUwopjTZj5XyZNOBcbJiyDSx6jPyeh14G2f5UNrTw_9xeOxDmz9EswZIoftu2tQO4SELaep7wjVawdK9jOU8JXzV5MDAZJBv4F6e00ZWEVa5aOMOHEJaiNj_pMXD722hZJDVYXhiUkFCT6EoOd1tPNzAJc4dzUZLYRKY9BALGmOH6Yz6pySAwCr7q5_pYCtDx0jyUhwLK7ywLRVwPX0uoeH_1ye5btUxTXAoP1g4tMzqyqaqGVfpi6yRtE0yTFz2TklGRpZNWO7pQ==&amp;xkcb=SoBp-_M3QegCKEWxBB0PbzkdCdPP&amp;p=2&amp;fvj=1&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>Acumatica (ERP) System Administrator</t>
+  </si>
+  <si>
+    <t>LHH Recruitment Solutions</t>
+  </si>
+  <si>
+    <t>New York, NY</t>
   </si>
   <si>
     <t>$90,000 - $120,000 a year
 Full-time</t>
   </si>
   <si>
-    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0A0FYroooRhadhP7IC5tdm37Ufrv5gQwUKA3VezZ1uuKrHGwi40GNW7lhuQF4GzPXVFQmvA8RWtOVcW5dYjt_EfedT-pJMRX1A-62CeawAWCO-CfeQT_1rSy8lAF2BClXKZ-oYJliTfXPmq9XdSMlttD9RA85cbIYTYLeb4Cprt1s9_A0pNrMobxvMfu5r_nRDcolkCkxckiLVZjz9WdkCRd0qMP9CD4QRcI9JqHrLvQVvWFP5TZ1DLVHOAbZnegq5CAl5FoQWH_NM0nPlzQjLHuurqxzthHR2-XYy7llVlDHvh2gZyx8xvRTVfD1utcFFnIpnpxd0-hskyuLF2T-eNotLZK59R_ehuMOcf-Ci9erICxk3DmCmvEVd0MKn-wj3Tdq2D-LT51j9NJI-Y8KcOLGd5TsgvfQy4rHdip2-vaVZOuONO8W2iHZPeKdKG5BW_h0qnHxYGjDcTaxHu9M-3-weIThcQlY8LopAE6PQxL_SF90xuk-WC3mGuOTCV_9mxrx6OpcZwICxDkXgiU0Orj9Lv5JhiHy2m3PSnZ3hKbLFL1PKa48Hm7aZ1SsTmFoTcoBYG6HhwvM4p_qY_PBE2rXmziuS1jFmBTcgwz2rbREK2vdaOvDONlDC-eWk5sdI=&amp;xkcb=SoD7-_M3Qd5AiLQgXJ0KbzkdCdPP&amp;p=1&amp;fvj=0&amp;vjs=3</t>
+    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0A_GD1K3dzeu7WcKnsm6RLSD1_QV-mkIht0EvhowBp1RB3nB2zK51B7Vjdo850qtD3HKWVgIj7fbhbwdbqxycFa0Fq8FmXoiogS7lCM9QVoCdq6EkjSA_6_dtfcjectZO7cvahtAQh2I0B3zGI4CU1cLtZLa7UmyuUN28cQHciW5X6f4opTNYHnn0RBz6CbUl4p8AcRuv0iOfIiyKVY9I7WKrbYhmxMa_OGkcXwCuiiZDbPVrdRuocxU7eqY2fSHskWS6mE4HKWsWOoWlv_3a8vfJtY3PGrZ75SsPRxvEeQNJriJxFSdmhlUO5Io6RPGxeSvbX8QrWqWZfjxY_ojluucfW16RDDrPfxCSTqdi0Age8jCgKH_fNupxdSR6hvogNXfK4-sk1fFVWzsiezVLZzF27C84hlQiKwvcib3HTzjvF8MssAaBbN8ASM1EhM8ye0vl-OpU0_LqkgdXrScWnbfZQW9L65H1VnbaxGDFDWCkRBzTvHPvjdp8Z4OB56HvHvbdPIhOpbu3cdZc41K0vz-6_8DaS7vhMKKwgSmXx755ly2Cw3W4fuqsygeXrVAWUId8ZC1NZvtZdE3lDegN-Ls5gMQHQW5FE_8KNOcXYeHgb6mz372-FyY9npMIrTsgln_opeOnxqZSRnLHDtCO7-bZ9HbEeA9j01mrpF8mWCcNKahZAL7oYtrLiUg0v5unrox15QFhIb3nSFiAdRJpNc5Dd9c4q2ii2lLYdCwC-Mtt5ZOaHd2U4xaEpHgouZCdmipKb8tkQTLA==&amp;xkcb=SoDd-_M3QegCKEWxBB0ObzkdCdPP&amp;p=3&amp;fvj=0&amp;vjs=3</t>
   </si>
   <si>
     <t>Systems Engineer with Windows Admin experience</t>
@@ -82,32 +112,26 @@
 +3</t>
   </si>
   <si>
-    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0Boequf9QJNUeapr-5YRE8VQe-jsUMvxvSbyJpb9cTUnsJKHh3xkSpesekGy6AkL_enFdksm3gFfT_QKHUZJES7cv9CVSCsfp6GrAgGyTcAjD-YnZZAIFbkQlk8DWVahWzdmuCdi6ykER4GvIe_zXp6UjsnECmF8vSyQ_KTKZHxDohlM7yrxsZteU6RUf69debjDWIljQrm1Lzxpe6SHofIX3xp6z94Rdu972WzvFNnr-jCOTBvybkzaRwSAzL_cRh_H_6XjYVN4J-ByNZXhokYAWfs3kktRVc_hkAuvS6-msOq3uRLe3wEEJhTiDfoyIiOCMSyFsqh4txJW9NfnjjVgkFg0k2gzO4xgPSBhAfn7BiafrLtgyBcbssqyFK2snRTvDpoH81IvUPDXisND1ILVFqfQLs2IJTOsHZXnnvgIsCmVRjXH9hKP8F1ChHaagEkugfgxecAzx54eTct5Q31ehqFRqKbluqn3SO2OC8OvQJTsv3NzOFUWMXYwe7izr1SuuHC5Moqa79SVW0drKUd4E9szYDsqr6-jT6KjeY97_8qOiI5bZitQvS08EEHX2Vm5ANx_V1WS-jlUUqgdEhp&amp;xkcb=SoBm-_M3Qd5AiLQgXJ0JbzkdCdPP&amp;p=2&amp;fvj=1&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>System Administrator</t>
-  </si>
-  <si>
-    <t>CyberCoders</t>
-  </si>
-  <si>
-    <t>Irvington, NY 10533</t>
-  </si>
-  <si>
-    <t>$75,000 - $110,000 a year
-Full-time</t>
-  </si>
-  <si>
-    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CpFJQzrgRR8WqXWK1qKKEqALWJw739KlKqr2H-MSI4eoBlI4EFrmor2FYZMP3muM2yJ85DoWTW6nYSz9x8yxVh9dNeQJ-WWlUHkbgE8cZix2VtfRF0JkDHz7v3HydoNe0VcjHbCsiXKhZJgwaL06EVImkIHFe8MzwJazUbKUkhXlZaVOyes6h_SNgLJTfFfAK6WEdRrC2yBWJZFrjBz-20IjrAACHA_XXZYDXkIv_UMlEkFxC-rqLzqPLosjrd4OVSiqW9mdIqymN5-VgryiatxBRSerOXylXZX9xXNpZNsX8x2C_7TstVGPhl_KJ9c_s4g_HRmUNAR3xs4Z8puJddAYEEAmz27xRo59PE5YUUdur9bPNBrPUf3dKZS7Rgrl8IY0xTQaKwPKWKAhAbGjp6k_iMQxhSH8xWN_Gut69NlOFCeXM5egx36Cz90sGZnWLNDQI5drVzY4VDCBhMWfIYXv1hQsstiZZC_0XPzq3by_4WrkVgsiPKJZkf8WdOIlLcWzKU2Tp6KYmry7UKm2J8k-mOUCIVvj4HbbOHqYRrV3jzM5wTqM5i6glUZ_Om5MhZ4lDhA19W68o58tlwlTmC-3PNUyG1enNrYNw0IxmdHHEDoJT-GjlgssmPhg9aC1BwF9PMFagnRTaicX906LzVZze-4TcqHpCUMl1MZzLHGz8uIeHpjxh9xYfFzc2wUDu9G5DQdZRY2m6CUzzGPm17sbgQrjAKczF_omllfCIjVDSloxs9m6Iqd-3X6uZEhIVT4BS-jfwDXfAkN5RnrqY-1NuvY8mwiX2U6XX-Jzg9WNHK6chVneAMP_rFVPvc9gP8AV4vt8uI8yQVL9he5GrqKoKKrfSieqXB5DJQriljMgpBtp_8s12h6WGAEGsSjXLHmipdWgFQnqiNaHV5vb9pbJaNpSykhhv-6CExZ8HtlQRa0REu5l6YELHe1TAyAWTUuVwsCxfZFfFaOqaJmTFTGa12cYZbvdQxa6ScAbzB_qBgPViwNue00ZZx_YdnFRw0ZOLs2-2YL-OVnTxjKyWh6Sh4s01w-aKwmFM8B3mvfziJmSDRs8dCRg9IDVT77u0QH6AArZDDatzvkE2lg1iXZ9Nksppx303RiF7MYYB2W5Y-Xq5izLsktJX-9RxBzBk=&amp;xkcb=SoDS-_M3Qd5AiLQgXJ0IbzkdCdPP&amp;p=3&amp;fvj=0&amp;vjs=3</t>
+    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0Boequf9QJNUeapr-5YRE8VQe-jsUMvxvSbyJpb9cTUnsJKHh3xkSpesekGy6AkL_enFdksm3gFfT_QKHUZJES7cv9CVSCsfp6GrAgGyTcAjD-YnZZAIFbkQlk8DWVahWzdmuCdi6ykER4GvIe_zXp6UjsnECmF8vSyQ_KTKZHxDmuiUPaef66gmQ9Vzl6mRW9MeqYElVdqef6mnmweoM315tJ9i1gjfdtAKYXb-fJbEfBJm05wHuHEmoS9tvyMDfPkZ2CcUnbas8dqSSMi-j1CXYPQCbRiCelrgAz6lOr-925IX52Hp-wi6nsNJ5xedlafsma0X9hQihmY8-CKEPNNzjJ9XfLty2UqjkEO6brDJrgGXfy0miuWHgeXP1uOfcK_L9Ow_9d2brzUaibUZySVkJmWkOXswVtzAgbNvP4nG3n-vhMZlN-r4q4ZVPpjWgY2b0-JLZfcwBCZ9fqUCKDxqQJj56smeV6Bes1WLRjj8LwZ1jn0dSRXlUAwTSwYelS0XFrvadxZX9wE-yYYLjAE5U46st5lDcPqtbF8exqzZk8t1p6PQ6B25aYGb9YAPAHIvNxjE8lJ9jC2-L3nm3JH&amp;xkcb=SoBA-_M3QegCKEWxBB0NbzkdCdPP&amp;p=4&amp;fvj=1&amp;vjs=3</t>
+  </si>
+  <si>
+    <t>vCIO / Managed Services System Administrator</t>
+  </si>
+  <si>
+    <t>Bowman Williams</t>
+  </si>
+  <si>
+    <t>New York, NY
++2 locations</t>
+  </si>
+  <si>
+    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0A0FYroooRhadhP7IC5tdm37Ufrv5gQwUKA3VezZ1uuKrHGwi40GNW7lhuQF4GzPXVFQmvA8RWtOVcW5dYjt_EfedT-pJMRX1A-62CeawAWCO-CfeQT_1rSy8lAF2BClXKZ-oYJliTfXPmq9XdSMlttD9RA85cbIYTYLeb4Cprt1s9_A0pNrMobxvMfu5r_nRDcolkCkxckiLVZjz9WdkCRyXXKkzdsvyAQOg0D00QR-lLTKq7DRtSHtMCRlL8l-_f_pYo9SWazMwPStX2gsrCN1HG7QowRzTUti1x08ZxotHZ7OYCkT0I6tjQJ0dblYADAZDByD8vDsQS5I5M354c0ct08gDb0bsWKyt10qBanGQ9W_Qnw4IpAiGPYdVLMWgNDQhbzaIr4he2iM3z7TbYoMzTtxX5gtvcPx9rtOD6-1iYPCHG0figmDM3rTdhsYfSHWjRVB3d4SHFXziGUCQPW1xjvc0xE_9R0tI9NpvSPRyL7lvdmyJRdp4VocqS7csFUD5GdrTv__CJU-3KjXEiA5sfVOYCagPQ8mPRewa_5RKU8c877M_oi4hKgMWtSVcbXnWZZ2weXOKlwpp4tA2jm57pU-vwU1tyWAWeWI3-YQeDbV-uOhitY9q0evz_0AHU=&amp;xkcb=SoD0-_M3QegCKEWxBB0MbzkdCdPP&amp;p=5&amp;fvj=0&amp;vjs=3</t>
   </si>
   <si>
     <t>Network Administrator</t>
   </si>
   <si>
     <t>Accenture</t>
-  </si>
-  <si>
-    <t>New York, NY</t>
   </si>
   <si>
     <t>$110,200 - $137,800 a year
@@ -165,6 +189,22 @@
     <t>https://www.indeed.com/rc/clk?jk=5d050727a88744ad&amp;fccid=7d7b563c6a3a9653&amp;vjs=3</t>
   </si>
   <si>
+    <t>System Administrator</t>
+  </si>
+  <si>
+    <t>CyberCoders</t>
+  </si>
+  <si>
+    <t>Irvington, NY 10533</t>
+  </si>
+  <si>
+    <t>$75,000 - $110,000 a year
+Full-time</t>
+  </si>
+  <si>
+    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CpFJQzrgRR8WqXWK1qKKEqALWJw739KlKqr2H-MSI4eoBlI4EFrmor2FYZMP3muM2yJ85DoWTW6nYSz9x8yxVh9dNeQJ-WWlUHkbgE8cZix2VtfRF0JkDHz7v3HydoNe0VcjHbCsiXKhZJgwaL06EVImkIHFe8MzwJazUbKUkhXkSUAoVjIEmYEc8j11yLraGtNjdahqf6ByVrzwEUnjq-VeVwl82VvVj36-DEDUjTE6QtDKLltjRXeqhifyoRHTbxRt21237GcQwTTxaXsmAtathi8YzWXGKSdSsdTfzi7Sa93zoPiVuRYBOTuqkfjPokH-ScLvcNXoGJzhuWD1Trc62_U-26uVJSHZ-jyqI04BGFl7qolOyNFiY98NvPDUl7xpEwF1J6U8-7XePNxs5i1a9YQXizH6p2P-GuNGq0txhzGMG1ni0dwwog4-nY-_oqOHAMRt6KbI5ZVgzZYd4AAkACGww5H-_gqEuSyrSa6xC1zFp_akm9fcgr3ggxbck1iJopJQF0t4-5LpAviNKEI_RY4nxRkiCuKPYnh8uUE5aHAGVajAxVDRfPZyq1nHTxEDohnmcS17kYO6bZ0DC8u5bROeZ92MfVtWRF0Ek5qG4P8hRJTAp0eNGYLNocZYtWB4UFMxbe_ALcjLWeOeFR1wTfNWIgW7SZTq2Op_qGHkb5-0mPxVI-rPGnG80yrbY9CTSW_-mSFWe5S3C6D7WZCcg4q72Av-gIzvu-Sxj650YkMgk_4gYmosKrC2DqWsDDN2_h9tk4SG0ozHFCihebrmwVUng5FeZfbXKb5rB6zHmcpzmB4YaNPWpVPmF6V4bmQpIx4mXyApDIDsipg1juZnLAvyMHBVPgU3Qb6JwCZS0QHGe1ZmOVSwwLdBwmeTRxeljQiVPs_IR5yISGtICiYLMoVq94sudM0pTk5EPrW3fNrxk9-M7D4ZMDJKt7B_AJeNSg7T9dUhK7oqOhWH5sytx52lrtuzaOf-EeguU5H6jYez9X7mb0p5htDmEVrUY37lB8TxlBxbDStmfdgj4Oq8ROCm2CjH3WHoD9xg4afxEnrUREiH3efN-aaDtDrKtxpxEMlWL8twwiHfNxHIe8IzndQaqKTXM8zi3PklOHkdnZ_Q0YPTKPvHEpH3ZHhb8=&amp;xkcb=SoAO-_M3QegCKEWxBB0HbzkdCdPP&amp;p=10&amp;fvj=0&amp;vjs=3</t>
+  </si>
+  <si>
     <t>Sr System Admin with Perl (C)</t>
   </si>
   <si>
@@ -192,53 +232,6 @@
     <t>https://www.indeed.com/company/Stone-Alliance-Group/jobs/IT-Administrator-fd1a281195b107b3?fccid=0ad0b184ba42375d&amp;vjs=3</t>
   </si>
   <si>
-    <t>NYC Careers</t>
-  </si>
-  <si>
-    <t>$85,371 - $119,883 a year
-Full-time
-Day shift</t>
-  </si>
-  <si>
-    <t>https://www.indeed.com/rc/clk?jk=8e42bfbec8c50971&amp;fccid=7d7b563c6a3a9653&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>System Admin - Level II support</t>
-  </si>
-  <si>
-    <t>Techresourcers</t>
-  </si>
-  <si>
-    <t>New York, NY 10007 
-(Tribeca area)</t>
-  </si>
-  <si>
-    <t>$90,000 - $95,000 a year
-Full-time</t>
-  </si>
-  <si>
-    <t>https://www.indeed.com/company/Techresourcers/jobs/Systems-Administrator-c070232c79158ec2?fccid=908613c0682a5bde&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>Windows System Administrator</t>
-  </si>
-  <si>
-    <t>Asset Inventories, Inc.</t>
-  </si>
-  <si>
-    <t>New York, NY 10022 
-(Midtown area)</t>
-  </si>
-  <si>
-    <t>$94,087 - $103,055 a year
-Full-time
-Monday to Friday
-+2</t>
-  </si>
-  <si>
-    <t>https://www.indeed.com/company/Asset-Inventories,-Inc./jobs/Systems-Administrator-ae1e17fb446e151a?fccid=99c1e13dccdcc2b3&amp;vjs=3</t>
-  </si>
-  <si>
     <t>Vinsys Inc</t>
   </si>
   <si>
@@ -254,23 +247,21 @@
     <t>https://www.indeed.com/company/Winsys-Information-Technology-Inc/jobs/Systems-Administrator-82cb08934c412eb8?fccid=b9d2c32181307a97&amp;vjs=3</t>
   </si>
   <si>
-    <t>IT Project Administrator</t>
-  </si>
-  <si>
-    <t>Pacer Staffing</t>
-  </si>
-  <si>
-    <t>Woodcliff Lake, NJ 07677</t>
-  </si>
-  <si>
-    <t>$47.25 an hour
-Full-time
-+1
-Monday to Friday
-+2</t>
-  </si>
-  <si>
-    <t>https://www.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0C9NbM5eTIyBy5lsQEfjp0LiR4ZnSOO0g4plUqowSZMmwKNhg9sK_ssyMkRY9ssskz5mu8YAXQZSyOP_yh85ADvhkXoW5nF3aGjWDHOdAy11FFW_9-P86n1ZaeLymI6IeCUnT5WwcsyKaNAzR9-qV1KaQLWD0kkwa5VrMA0x8z-ef7nqgKMNLX5kIneE5N2HeXpWBgAkYbz-V9Ehnh8R4afvM2FHdgsTnNKGs1wYqBakqICYSrRW_nazCn7gMUYpc93NDc-VURfw1liXd4WnlIQ1vDkp8Kd_SQNEAG9eNM3GQWcZgiIpWvp67vtwtMUgY3X0UV5nH4iKoaZKw4VNgUXV3FaOZjLdH3ThNoeT-Tf6jSvKnAfPIKLeVz74d8j5e3fXghdQajAcdJzXocd1Ut9sfHQpU7ql7emEueu-qFF6p9rrJ8Jd4oOJNaEK-984OBcuKRkVDet1b7tV49pnAd4QkPQXoYXcQ4l03TX-QU982jIpVSEzTPVFTR4myWmcunq-j43z_Kh6pOwL6B7fLO0Lhh-k9_ZorTPHNPfkLTvN7Lwv4WQFiAL6mXjKaPejxK05fWbsXqxBA==&amp;xkcb=SoAS-_M3Qd5AiLQgXJ0FbzkdCdPP&amp;p=14&amp;fvj=1&amp;vjs=3</t>
+    <t>System Admin - Level II support</t>
+  </si>
+  <si>
+    <t>Techresourcers</t>
+  </si>
+  <si>
+    <t>New York, NY 10007 
+(Tribeca area)</t>
+  </si>
+  <si>
+    <t>$90,000 - $95,000 a year
+Full-time</t>
+  </si>
+  <si>
+    <t>https://www.indeed.com/company/Techresourcers/jobs/Systems-Administrator-c070232c79158ec2?fccid=908613c0682a5bde&amp;vjs=3</t>
   </si>
 </sst>
 </file>
@@ -669,163 +660,163 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
         <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>53</v>
@@ -842,64 +833,64 @@
         <v>56</v>
       </c>
       <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
         <v>61</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>